<commit_message>
pr7 + pr6 algo done, pr2 arch almost done
</commit_message>
<xml_diff>
--- a/Achitech/tables/PR_2_michel.xlsx
+++ b/Achitech/tables/PR_2_michel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\Achitech\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Uni\Files\Uni_docs\Achitech\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0139765-FC48-4D65-9906-4B97EC6253A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF2B3C7-2762-4F7F-91B6-1B8F535EDA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9045" yWindow="480" windowWidth="28680" windowHeight="15345" activeTab="2" xr2:uid="{6AF5EB4D-14FB-41EF-A5B1-3017AA22F430}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" activeTab="1" xr2:uid="{6AF5EB4D-14FB-41EF-A5B1-3017AA22F430}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="91">
   <si>
     <t>№</t>
   </si>
@@ -440,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -464,23 +464,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -495,7 +488,14 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -552,9 +552,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office 2013–2022">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -592,7 +592,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -698,7 +698,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -840,7 +840,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -851,43 +851,43 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:C25"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.53515625" customWidth="1"/>
+    <col min="2" max="2" width="4.84375" customWidth="1"/>
+    <col min="3" max="3" width="11.3828125" customWidth="1"/>
     <col min="4" max="4" width="6" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.3828125" customWidth="1"/>
+    <col min="6" max="6" width="6.15234375" customWidth="1"/>
+    <col min="7" max="7" width="12.3828125" customWidth="1"/>
+    <col min="9" max="9" width="11.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="75.75" thickBot="1">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:16" ht="74.150000000000006" thickBot="1">
+      <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16" t="s">
+      <c r="B1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="16" t="s">
+      <c r="F1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16" t="s">
+      <c r="H1" s="13"/>
+      <c r="I1" s="13" t="s">
         <v>2</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -909,28 +909,28 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="19.5" thickBot="1">
-      <c r="A2" s="17">
-        <v>1</v>
-      </c>
-      <c r="B2" s="17">
-        <v>1</v>
-      </c>
-      <c r="C2" s="17" t="s">
+    <row r="2" spans="1:16" ht="18.899999999999999" thickBot="1">
+      <c r="A2" s="14">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14">
+        <v>1</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17" t="s">
+      <c r="D2" s="14"/>
+      <c r="E2" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="17">
-        <v>1</v>
-      </c>
-      <c r="G2" s="17" t="s">
+      <c r="F2" s="14">
+        <v>1</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17" t="s">
+      <c r="H2" s="14"/>
+      <c r="I2" s="14" t="s">
         <v>88</v>
       </c>
       <c r="K2" s="3">
@@ -952,26 +952,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="19.5" thickBot="1">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17">
+    <row r="3" spans="1:16" ht="18.899999999999999" thickBot="1">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14">
         <v>2</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17" t="s">
+      <c r="D3" s="14"/>
+      <c r="E3" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="14">
         <v>2</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17" t="s">
+      <c r="H3" s="14"/>
+      <c r="I3" s="14" t="s">
         <v>89</v>
       </c>
       <c r="K3" s="3">
@@ -993,26 +993,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="19.5" thickBot="1">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17">
+    <row r="4" spans="1:16" ht="18.899999999999999" thickBot="1">
+      <c r="A4" s="14"/>
+      <c r="B4" s="14">
         <v>3</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="14">
         <v>10000</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17" t="s">
+      <c r="D4" s="14"/>
+      <c r="E4" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="14">
         <v>3</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
       <c r="K4" s="3">
         <v>0</v>
       </c>
@@ -1032,16 +1032,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="19.5" thickBot="1">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
+    <row r="5" spans="1:16" ht="18.899999999999999" thickBot="1">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
       <c r="K5" s="3">
         <v>0</v>
       </c>
@@ -1061,28 +1061,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="19.5" thickBot="1">
-      <c r="A6" s="17">
+    <row r="6" spans="1:16" ht="18.899999999999999" thickBot="1">
+      <c r="A6" s="14">
         <v>2</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="14">
         <v>4</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17" t="s">
+      <c r="D6" s="14"/>
+      <c r="E6" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="14">
         <v>4</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
       <c r="K6" s="3">
         <v>0</v>
       </c>
@@ -1102,24 +1102,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="19.5" thickBot="1">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17" t="s">
+    <row r="7" spans="1:16" ht="18.899999999999999" thickBot="1">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17" t="s">
+      <c r="D7" s="14"/>
+      <c r="E7" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="14">
         <v>5</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
       <c r="K7" s="3">
         <v>0</v>
       </c>
@@ -1139,24 +1139,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="19.5" thickBot="1">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17" t="s">
+    <row r="8" spans="1:16" ht="18.899999999999999" thickBot="1">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17" t="s">
+      <c r="D8" s="14"/>
+      <c r="E8" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="14">
         <v>6</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
       <c r="K8" s="3">
         <v>0</v>
       </c>
@@ -1176,26 +1176,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="19.5" thickBot="1">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17">
+    <row r="9" spans="1:16" ht="18.899999999999999" thickBot="1">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14">
         <v>5</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17" t="s">
+      <c r="D9" s="14"/>
+      <c r="E9" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="14">
         <v>7</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
       <c r="K9" s="3">
         <v>0</v>
       </c>
@@ -1215,24 +1215,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="19.5" thickBot="1">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17" t="s">
+    <row r="10" spans="1:16" ht="18.899999999999999" thickBot="1">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17" t="s">
+      <c r="D10" s="14"/>
+      <c r="E10" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="14">
         <v>8</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
       <c r="K10" s="3">
         <v>0</v>
       </c>
@@ -1252,26 +1252,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="19.5" thickBot="1">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17">
+    <row r="11" spans="1:16" ht="18.899999999999999" thickBot="1">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14">
         <v>6</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17" t="s">
+      <c r="D11" s="14"/>
+      <c r="E11" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="14">
         <v>9</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
       <c r="K11" s="3">
         <v>0</v>
       </c>
@@ -1291,24 +1291,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="19.5" thickBot="1">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17" t="s">
+    <row r="12" spans="1:16" ht="18.899999999999999" thickBot="1">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17" t="s">
+      <c r="D12" s="14"/>
+      <c r="E12" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="14">
         <v>10</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
       <c r="K12" s="3">
         <v>0</v>
       </c>
@@ -1328,26 +1328,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="19.5" thickBot="1">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17">
+    <row r="13" spans="1:16" ht="18.899999999999999" thickBot="1">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14">
         <v>7</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="14">
         <v>10100</v>
       </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17" t="s">
+      <c r="D13" s="14"/>
+      <c r="E13" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="14">
         <v>11</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
       <c r="K13" s="3">
         <v>0</v>
       </c>
@@ -1367,22 +1367,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="19.5" thickBot="1">
-      <c r="A14" s="17">
+    <row r="14" spans="1:16" ht="18.899999999999999" thickBot="1">
+      <c r="A14" s="14">
         <v>3</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
       <c r="K14" s="3">
         <v>0</v>
       </c>
@@ -1402,16 +1402,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="19.5" thickBot="1">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
+    <row r="15" spans="1:16" ht="18.899999999999999" thickBot="1">
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
       <c r="K15" s="3">
         <v>0</v>
       </c>
@@ -1431,26 +1431,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="19.5" thickBot="1">
-      <c r="A16" s="18"/>
-      <c r="B16" s="17">
+    <row r="16" spans="1:16" ht="18.899999999999999" thickBot="1">
+      <c r="A16" s="15"/>
+      <c r="B16" s="14">
         <v>9</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17" t="s">
+      <c r="D16" s="14"/>
+      <c r="E16" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="G16" s="17">
+      <c r="G16" s="14">
         <v>-1101</v>
       </c>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
       <c r="K16" s="3">
         <v>0</v>
       </c>
@@ -1470,26 +1470,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="19.5" thickBot="1">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17">
+    <row r="17" spans="1:16" ht="18.899999999999999" thickBot="1">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14">
         <v>10</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17" t="s">
+      <c r="D17" s="14"/>
+      <c r="E17" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="G17" s="17">
+      <c r="G17" s="14">
         <v>-1110</v>
       </c>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
       <c r="K17" s="3">
         <v>0</v>
       </c>
@@ -1509,26 +1509,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="19.5" thickBot="1">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17">
+    <row r="18" spans="1:16" ht="18.899999999999999" thickBot="1">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14">
         <v>11</v>
       </c>
-      <c r="C18" s="17">
+      <c r="C18" s="14">
         <v>10011</v>
       </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17" t="s">
+      <c r="D18" s="14"/>
+      <c r="E18" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="F18" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="G18" s="17" t="s">
+      <c r="G18" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
       <c r="K18" s="3">
         <v>1</v>
       </c>
@@ -1548,28 +1548,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="19.5" thickBot="1">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17">
+    <row r="19" spans="1:16" ht="18.899999999999999" thickBot="1">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14">
         <v>12</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17" t="s">
+      <c r="D19" s="14"/>
+      <c r="E19" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="G19" s="17" t="s">
+      <c r="G19" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H19" s="17" t="s">
+      <c r="H19" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="I19" s="17"/>
+      <c r="I19" s="14"/>
       <c r="K19" s="3">
         <v>1</v>
       </c>
@@ -1589,22 +1589,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="19.5" thickBot="1">
-      <c r="A20" s="17">
+    <row r="20" spans="1:16" ht="18.899999999999999" thickBot="1">
+      <c r="A20" s="14">
         <v>4</v>
       </c>
-      <c r="B20" s="17">
+      <c r="B20" s="14">
         <v>13</v>
       </c>
-      <c r="C20" s="17">
+      <c r="C20" s="14">
         <v>11011</v>
       </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
       <c r="K20" s="3">
         <v>1</v>
       </c>
@@ -1624,20 +1624,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="19.5" thickBot="1">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17">
+    <row r="21" spans="1:16" ht="18.899999999999999" thickBot="1">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14">
         <v>14</v>
       </c>
-      <c r="C21" s="17">
+      <c r="C21" s="14">
         <v>11101</v>
       </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
       <c r="K21" s="3">
         <v>1</v>
       </c>
@@ -1657,22 +1657,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="19.5" thickBot="1">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17">
+    <row r="22" spans="1:16" ht="18.899999999999999" thickBot="1">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14">
         <v>15</v>
       </c>
-      <c r="C22" s="17">
+      <c r="C22" s="14">
         <v>11110</v>
       </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17" t="s">
+      <c r="D22" s="14"/>
+      <c r="E22" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
       <c r="K22" s="3">
         <v>1</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15.75" thickBot="1">
+    <row r="23" spans="1:16" ht="15" thickBot="1">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1721,7 +1721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15.75" thickBot="1">
+    <row r="24" spans="1:16" ht="15" thickBot="1">
       <c r="A24" s="7" t="s">
         <v>53</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15.75" thickBot="1">
+    <row r="25" spans="1:16" ht="15" thickBot="1">
       <c r="A25" s="7"/>
       <c r="B25" s="7" t="s">
         <v>53</v>
@@ -1789,7 +1789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="15.75" thickBot="1">
+    <row r="26" spans="1:16" ht="15" thickBot="1">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1818,7 +1818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="15.75" thickBot="1">
+    <row r="27" spans="1:16" ht="15" thickBot="1">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -1847,7 +1847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="15.75" thickBot="1">
+    <row r="28" spans="1:16" ht="15" thickBot="1">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -1878,7 +1878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15.75" thickBot="1">
+    <row r="29" spans="1:16" ht="15" thickBot="1">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -1907,7 +1907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="15.75" thickBot="1">
+    <row r="30" spans="1:16" ht="15" thickBot="1">
       <c r="K30" s="3">
         <v>1</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="15.75" thickBot="1">
+    <row r="31" spans="1:16" ht="15" thickBot="1">
       <c r="K31" s="3">
         <v>1</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="15.75" thickBot="1">
+    <row r="32" spans="1:16" ht="15" thickBot="1">
       <c r="K32" s="3">
         <v>1</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="11:16" ht="15.75" thickBot="1">
+    <row r="33" spans="11:16" ht="15" thickBot="1">
       <c r="K33" s="3">
         <v>1</v>
       </c>
@@ -1990,7 +1990,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="K2:P33">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>$P2=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2001,15 +2001,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99FB2CE3-59A1-4918-BBB6-4D375F3C51EB}">
-  <dimension ref="A1:U33"/>
+  <dimension ref="A1:Z33"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection sqref="A1:P18"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:26">
       <c r="A1" s="8"/>
       <c r="B1" s="8"/>
       <c r="C1" s="8" t="s">
@@ -2055,12 +2055,31 @@
         <v>83</v>
       </c>
       <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-    </row>
-    <row r="2" spans="1:21">
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="X1" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y1" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8" t="s">
@@ -2106,12 +2125,31 @@
         <v>52</v>
       </c>
       <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-    </row>
-    <row r="3" spans="1:21">
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="V2" s="8">
+        <v>-1101</v>
+      </c>
+      <c r="W2" s="8">
+        <v>-1110</v>
+      </c>
+      <c r="X2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z2" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8" t="s">
@@ -2139,12 +2177,21 @@
       <c r="O3" s="8"/>
       <c r="P3" s="11"/>
       <c r="Q3" s="9"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-    </row>
-    <row r="4" spans="1:21">
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="X3" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="11"/>
+    </row>
+    <row r="4" spans="1:26">
       <c r="A4" s="8" t="s">
         <v>55</v>
       </c>
@@ -2171,12 +2218,21 @@
         <f>SUM(C4:P4)</f>
         <v>1</v>
       </c>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-    </row>
-    <row r="5" spans="1:21">
+      <c r="R4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="S4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="11"/>
+    </row>
+    <row r="5" spans="1:26">
       <c r="A5" s="8" t="s">
         <v>56</v>
       </c>
@@ -2203,12 +2259,21 @@
         <f t="shared" ref="Q5:Q18" si="0">SUM(C5:P5)</f>
         <v>1</v>
       </c>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-    </row>
-    <row r="6" spans="1:21">
+      <c r="R5" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="S5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="11"/>
+    </row>
+    <row r="6" spans="1:26">
       <c r="A6" s="8" t="s">
         <v>57</v>
       </c>
@@ -2235,12 +2300,21 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-    </row>
-    <row r="7" spans="1:21">
+      <c r="R6" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="S6" s="8">
+        <v>10000</v>
+      </c>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="11"/>
+    </row>
+    <row r="7" spans="1:26">
       <c r="A7" s="8" t="s">
         <v>58</v>
       </c>
@@ -2271,12 +2345,23 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-    </row>
-    <row r="8" spans="1:21">
+      <c r="R7" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="S7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26">
       <c r="A8" s="8" t="s">
         <v>59</v>
       </c>
@@ -2305,12 +2390,21 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
-    </row>
-    <row r="9" spans="1:21">
+      <c r="R8" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="S8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="11"/>
+    </row>
+    <row r="9" spans="1:26">
       <c r="A9" s="8" t="s">
         <v>60</v>
       </c>
@@ -2341,12 +2435,23 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-    </row>
-    <row r="10" spans="1:21">
+      <c r="R9" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="S9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="T9" s="11">
+        <v>1</v>
+      </c>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="11"/>
+    </row>
+    <row r="10" spans="1:26">
       <c r="A10" s="8" t="s">
         <v>61</v>
       </c>
@@ -2375,12 +2480,23 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
-      <c r="U10" s="7"/>
-    </row>
-    <row r="11" spans="1:21">
+      <c r="R10" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="S10" s="8">
+        <v>10100</v>
+      </c>
+      <c r="T10" s="10"/>
+      <c r="U10" s="11">
+        <v>1</v>
+      </c>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="11"/>
+    </row>
+    <row r="11" spans="1:26">
       <c r="A11" s="8" t="s">
         <v>62</v>
       </c>
@@ -2409,12 +2525,21 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7"/>
-      <c r="U11" s="7"/>
-    </row>
-    <row r="12" spans="1:21">
+      <c r="R11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="S11" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="11"/>
+    </row>
+    <row r="12" spans="1:26">
       <c r="A12" s="8" t="s">
         <v>63</v>
       </c>
@@ -2445,12 +2570,25 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="7"/>
-      <c r="U12" s="7"/>
-    </row>
-    <row r="13" spans="1:21">
+      <c r="R12" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="S12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="11">
+        <v>1</v>
+      </c>
+      <c r="W12" s="10"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
       <c r="A13" s="8" t="s">
         <v>64</v>
       </c>
@@ -2481,12 +2619,25 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
-      <c r="U13" s="7"/>
-    </row>
-    <row r="14" spans="1:21">
+      <c r="R13" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="S13" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="T13" s="11">
+        <v>1</v>
+      </c>
+      <c r="U13" s="10"/>
+      <c r="V13" s="10"/>
+      <c r="W13" s="11">
+        <v>1</v>
+      </c>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="10"/>
+      <c r="Z13" s="11"/>
+    </row>
+    <row r="14" spans="1:26">
       <c r="A14" s="8" t="s">
         <v>65</v>
       </c>
@@ -2513,12 +2664,23 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="R14" s="7"/>
-      <c r="S14" s="7"/>
-      <c r="T14" s="7"/>
-      <c r="U14" s="7"/>
-    </row>
-    <row r="15" spans="1:21">
+      <c r="R14" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="S14" s="8">
+        <v>10011</v>
+      </c>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="10"/>
+      <c r="W14" s="10"/>
+      <c r="X14" s="11">
+        <v>1</v>
+      </c>
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="11"/>
+    </row>
+    <row r="15" spans="1:26">
       <c r="A15" s="8" t="s">
         <v>66</v>
       </c>
@@ -2549,12 +2711,27 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
-    </row>
-    <row r="16" spans="1:21">
+      <c r="R15" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="S15" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="T15" s="10"/>
+      <c r="U15" s="11">
+        <v>1</v>
+      </c>
+      <c r="V15" s="10"/>
+      <c r="W15" s="10"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="11">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
       <c r="A16" s="8" t="s">
         <v>67</v>
       </c>
@@ -2581,12 +2758,23 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
-      <c r="U16" s="7"/>
-    </row>
-    <row r="17" spans="1:21">
+      <c r="R16" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="S16" s="8">
+        <v>11011</v>
+      </c>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="10"/>
+      <c r="X16" s="11">
+        <v>1</v>
+      </c>
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="11"/>
+    </row>
+    <row r="17" spans="1:26">
       <c r="A17" s="8" t="s">
         <v>68</v>
       </c>
@@ -2617,12 +2805,27 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
-      <c r="T17" s="7"/>
-      <c r="U17" s="7"/>
-    </row>
-    <row r="18" spans="1:21">
+      <c r="R17" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="S17" s="8">
+        <v>11101</v>
+      </c>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="11">
+        <v>1</v>
+      </c>
+      <c r="W17" s="10"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="11">
+        <v>1</v>
+      </c>
+      <c r="Z17" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26">
       <c r="A18" s="8" t="s">
         <v>69</v>
       </c>
@@ -2649,12 +2852,23 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="R18" s="7"/>
-      <c r="S18" s="7"/>
-      <c r="T18" s="7"/>
-      <c r="U18" s="7"/>
-    </row>
-    <row r="21" spans="1:21">
+      <c r="R18" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="S18" s="8">
+        <v>11110</v>
+      </c>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="11">
+        <v>1</v>
+      </c>
+      <c r="X18" s="10"/>
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="11"/>
+    </row>
+    <row r="21" spans="1:26">
       <c r="A21" s="8" t="s">
         <v>11</v>
       </c>
@@ -2671,47 +2885,47 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:26">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:26">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:26">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:26">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:26">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
     </row>
-    <row r="27" spans="1:21">
+    <row r="27" spans="1:26">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
     </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:26">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:26">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:26">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:26">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
     </row>
-    <row r="32" spans="1:21">
+    <row r="32" spans="1:26">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
     </row>
@@ -2722,7 +2936,12 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C4:P18">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="5" priority="2">
+      <formula>$Q4=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T4:Z18">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$Q4=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2733,39 +2952,39 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D030BD7-E75B-43E4-833B-44F5C9225100}">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="12"/>
-      <c r="B1" s="12"/>
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
       <c r="C1" s="8" t="s">
         <v>74</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
       <c r="C2" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="8" t="s">
@@ -2778,9 +2997,9 @@
         <v>1</v>
       </c>
       <c r="D3" s="11"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="8" t="s">
@@ -2793,9 +3012,9 @@
         <v>1</v>
       </c>
       <c r="D4" s="11"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="8" t="s">
@@ -2808,9 +3027,9 @@
       <c r="D5" s="11">
         <v>1</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="14"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="8" t="s">
@@ -2823,9 +3042,9 @@
       <c r="D6" s="11">
         <v>1</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="15"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="8" t="s">
@@ -2838,7 +3057,7 @@
       <c r="D7" s="11">
         <v>1</v>
       </c>
-      <c r="E7" s="14"/>
+      <c r="E7" s="12"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="8" t="s">
@@ -2881,8 +3100,8 @@
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
       <c r="C14" s="8" t="s">
         <v>73</v>
       </c>
@@ -2912,8 +3131,8 @@
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
       <c r="C15" s="8" t="s">
         <v>14</v>
       </c>
@@ -2963,7 +3182,7 @@
       <c r="J16" s="10"/>
       <c r="K16" s="11"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:11">
       <c r="A17" s="8" t="s">
         <v>62</v>
       </c>
@@ -2984,7 +3203,7 @@
       <c r="J17" s="10"/>
       <c r="K17" s="11"/>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:11">
       <c r="A18" s="8" t="s">
         <v>63</v>
       </c>
@@ -3007,7 +3226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:11">
       <c r="A19" s="8" t="s">
         <v>66</v>
       </c>
@@ -3030,7 +3249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:11">
       <c r="A20" s="8" t="s">
         <v>68</v>
       </c>
@@ -3053,21 +3272,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="13"/>
+    <row r="24" spans="1:11">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="9"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C7:E7 C20:K20">
+    <cfRule type="expression" dxfId="4" priority="10">
+      <formula>$Q17=1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C3:G3 C16:K16">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>$Q8=1</formula>
@@ -3083,11 +3306,6 @@
       <formula>$Q15=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:E7 C20:K20">
-    <cfRule type="expression" dxfId="0" priority="10">
-      <formula>$Q17=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
doc8 chaged + doclad for algo code
</commit_message>
<xml_diff>
--- a/Achitech/tables/PR_2_michel.xlsx
+++ b/Achitech/tables/PR_2_michel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Uni\Files\Uni_docs\Achitech\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\Achitech\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF2B3C7-2762-4F7F-91B6-1B8F535EDA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2243D922-A992-4036-BF64-7FC7383D8B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" activeTab="1" xr2:uid="{6AF5EB4D-14FB-41EF-A5B1-3017AA22F430}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="2" xr2:uid="{6AF5EB4D-14FB-41EF-A5B1-3017AA22F430}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -552,9 +552,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office 2013–2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -592,7 +592,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -698,7 +698,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -840,7 +840,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -854,19 +854,19 @@
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.53515625" customWidth="1"/>
-    <col min="2" max="2" width="4.84375" customWidth="1"/>
-    <col min="3" max="3" width="11.3828125" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
     <col min="4" max="4" width="6" customWidth="1"/>
-    <col min="5" max="5" width="13.3828125" customWidth="1"/>
-    <col min="6" max="6" width="6.15234375" customWidth="1"/>
-    <col min="7" max="7" width="12.3828125" customWidth="1"/>
-    <col min="9" max="9" width="11.84375" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="74.150000000000006" thickBot="1">
+    <row r="1" spans="1:16" ht="75.75" thickBot="1">
       <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
@@ -909,7 +909,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="18.899999999999999" thickBot="1">
+    <row r="2" spans="1:16" ht="19.5" thickBot="1">
       <c r="A2" s="14">
         <v>1</v>
       </c>
@@ -952,7 +952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="18.899999999999999" thickBot="1">
+    <row r="3" spans="1:16" ht="19.5" thickBot="1">
       <c r="A3" s="14"/>
       <c r="B3" s="14">
         <v>2</v>
@@ -993,7 +993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="18.899999999999999" thickBot="1">
+    <row r="4" spans="1:16" ht="19.5" thickBot="1">
       <c r="A4" s="14"/>
       <c r="B4" s="14">
         <v>3</v>
@@ -1032,7 +1032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="18.899999999999999" thickBot="1">
+    <row r="5" spans="1:16" ht="19.5" thickBot="1">
       <c r="A5" s="15"/>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
@@ -1061,7 +1061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="18.899999999999999" thickBot="1">
+    <row r="6" spans="1:16" ht="19.5" thickBot="1">
       <c r="A6" s="14">
         <v>2</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="18.899999999999999" thickBot="1">
+    <row r="7" spans="1:16" ht="19.5" thickBot="1">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14" t="s">
@@ -1139,7 +1139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="18.899999999999999" thickBot="1">
+    <row r="8" spans="1:16" ht="19.5" thickBot="1">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14" t="s">
@@ -1176,7 +1176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="18.899999999999999" thickBot="1">
+    <row r="9" spans="1:16" ht="19.5" thickBot="1">
       <c r="A9" s="14"/>
       <c r="B9" s="14">
         <v>5</v>
@@ -1215,7 +1215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="18.899999999999999" thickBot="1">
+    <row r="10" spans="1:16" ht="19.5" thickBot="1">
       <c r="A10" s="14"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14" t="s">
@@ -1252,7 +1252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="18.899999999999999" thickBot="1">
+    <row r="11" spans="1:16" ht="19.5" thickBot="1">
       <c r="A11" s="14"/>
       <c r="B11" s="14">
         <v>6</v>
@@ -1291,7 +1291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="18.899999999999999" thickBot="1">
+    <row r="12" spans="1:16" ht="19.5" thickBot="1">
       <c r="A12" s="14"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14" t="s">
@@ -1328,7 +1328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="18.899999999999999" thickBot="1">
+    <row r="13" spans="1:16" ht="19.5" thickBot="1">
       <c r="A13" s="14"/>
       <c r="B13" s="14">
         <v>7</v>
@@ -1367,7 +1367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="18.899999999999999" thickBot="1">
+    <row r="14" spans="1:16" ht="19.5" thickBot="1">
       <c r="A14" s="14">
         <v>3</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="18.899999999999999" thickBot="1">
+    <row r="15" spans="1:16" ht="19.5" thickBot="1">
       <c r="A15" s="15"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -1431,7 +1431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="18.899999999999999" thickBot="1">
+    <row r="16" spans="1:16" ht="19.5" thickBot="1">
       <c r="A16" s="15"/>
       <c r="B16" s="14">
         <v>9</v>
@@ -1470,7 +1470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="18.899999999999999" thickBot="1">
+    <row r="17" spans="1:16" ht="19.5" thickBot="1">
       <c r="A17" s="14"/>
       <c r="B17" s="14">
         <v>10</v>
@@ -1509,7 +1509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="18.899999999999999" thickBot="1">
+    <row r="18" spans="1:16" ht="19.5" thickBot="1">
       <c r="A18" s="14"/>
       <c r="B18" s="14">
         <v>11</v>
@@ -1548,7 +1548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="18.899999999999999" thickBot="1">
+    <row r="19" spans="1:16" ht="19.5" thickBot="1">
       <c r="A19" s="14"/>
       <c r="B19" s="14">
         <v>12</v>
@@ -1589,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="18.899999999999999" thickBot="1">
+    <row r="20" spans="1:16" ht="19.5" thickBot="1">
       <c r="A20" s="14">
         <v>4</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="18.899999999999999" thickBot="1">
+    <row r="21" spans="1:16" ht="19.5" thickBot="1">
       <c r="A21" s="14"/>
       <c r="B21" s="14">
         <v>14</v>
@@ -1657,7 +1657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="18.899999999999999" thickBot="1">
+    <row r="22" spans="1:16" ht="19.5" thickBot="1">
       <c r="A22" s="14"/>
       <c r="B22" s="14">
         <v>15</v>
@@ -1692,7 +1692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15" thickBot="1">
+    <row r="23" spans="1:16" ht="15.75" thickBot="1">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1721,7 +1721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15" thickBot="1">
+    <row r="24" spans="1:16" ht="15.75" thickBot="1">
       <c r="A24" s="7" t="s">
         <v>53</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15" thickBot="1">
+    <row r="25" spans="1:16" ht="15.75" thickBot="1">
       <c r="A25" s="7"/>
       <c r="B25" s="7" t="s">
         <v>53</v>
@@ -1789,7 +1789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="15" thickBot="1">
+    <row r="26" spans="1:16" ht="15.75" thickBot="1">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1818,7 +1818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="15" thickBot="1">
+    <row r="27" spans="1:16" ht="15.75" thickBot="1">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -1847,7 +1847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="15" thickBot="1">
+    <row r="28" spans="1:16" ht="15.75" thickBot="1">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -1878,7 +1878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15" thickBot="1">
+    <row r="29" spans="1:16" ht="15.75" thickBot="1">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -1907,7 +1907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="15" thickBot="1">
+    <row r="30" spans="1:16" ht="15.75" thickBot="1">
       <c r="K30" s="3">
         <v>1</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="15" thickBot="1">
+    <row r="31" spans="1:16" ht="15.75" thickBot="1">
       <c r="K31" s="3">
         <v>1</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="15" thickBot="1">
+    <row r="32" spans="1:16" ht="15.75" thickBot="1">
       <c r="K32" s="3">
         <v>1</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="11:16" ht="15" thickBot="1">
+    <row r="33" spans="11:16" ht="15.75" thickBot="1">
       <c r="K33" s="3">
         <v>1</v>
       </c>
@@ -2003,11 +2003,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99FB2CE3-59A1-4918-BBB6-4D375F3C51EB}">
   <dimension ref="A1:Z33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
       <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="8"/>
@@ -2941,7 +2941,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T4:Z18">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$Q4=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2954,11 +2954,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D030BD7-E75B-43E4-833B-44F5C9225100}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="7"/>
@@ -3287,22 +3287,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C7:E7 C20:K20">
-    <cfRule type="expression" dxfId="4" priority="10">
+    <cfRule type="expression" dxfId="3" priority="10">
       <formula>$Q17=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:G3 C16:K16">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>$Q8=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:G5 C17:K18 C24:K24">
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="1" priority="6">
       <formula>$Q11=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:G6 C19:K19">
-    <cfRule type="expression" dxfId="1" priority="8">
+    <cfRule type="expression" dxfId="0" priority="8">
       <formula>$Q15=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>